<commit_message>
check again admin page
</commit_message>
<xml_diff>
--- a/excel_sheets/liste_allergies.xlsx
+++ b/excel_sheets/liste_allergies.xlsx
@@ -1,94 +1,91 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="liste_allergies_wand" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
+    <t>Spécificité</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Spécificité</t>
+    <t>Arachides</t>
   </si>
   <si>
     <t>Alimentaire</t>
   </si>
   <si>
+    <t>Fruits à coque (noix, amandes...)</t>
+  </si>
+  <si>
+    <t>Fruits de mer (crevettes, crabes...)</t>
+  </si>
+  <si>
+    <t>Lait de vache</t>
+  </si>
+  <si>
+    <t>Œufs</t>
+  </si>
+  <si>
+    <t>Blé (gluten)</t>
+  </si>
+  <si>
+    <t>Soja</t>
+  </si>
+  <si>
+    <t>Pollen (graminées, arbres)</t>
+  </si>
+  <si>
     <t>Respiratoire</t>
   </si>
   <si>
+    <t>Acariens</t>
+  </si>
+  <si>
+    <t>Poils d’animaux (chats, chiens)</t>
+  </si>
+  <si>
+    <t>Moisissures</t>
+  </si>
+  <si>
+    <t>Pénicilline</t>
+  </si>
+  <si>
     <t>Médicamenteuse</t>
   </si>
   <si>
+    <t>Aspirine (AINS)</t>
+  </si>
+  <si>
+    <t>Iode (produits de contraste)</t>
+  </si>
+  <si>
+    <t>Piqûres d’abeilles</t>
+  </si>
+  <si>
     <t>Insectes</t>
   </si>
   <si>
+    <t>Piqûres de guêpes</t>
+  </si>
+  <si>
+    <t>Piqûres de frelons</t>
+  </si>
+  <si>
+    <t>Latex</t>
+  </si>
+  <si>
     <t>Contact</t>
-  </si>
-  <si>
-    <t>Arachides</t>
-  </si>
-  <si>
-    <t>Fruits à coque (noix, amandes...)</t>
-  </si>
-  <si>
-    <t>Fruits de mer (crevettes, crabes...)</t>
-  </si>
-  <si>
-    <t>Lait de vache</t>
-  </si>
-  <si>
-    <t>Œufs</t>
-  </si>
-  <si>
-    <t>Blé (gluten)</t>
-  </si>
-  <si>
-    <t>Soja</t>
-  </si>
-  <si>
-    <t>Pollen (graminées, arbres)</t>
-  </si>
-  <si>
-    <t>Acariens</t>
-  </si>
-  <si>
-    <t>Poils d’animaux (chats, chiens)</t>
-  </si>
-  <si>
-    <t>Moisissures</t>
-  </si>
-  <si>
-    <t>Pénicilline</t>
-  </si>
-  <si>
-    <t>Aspirine (AINS)</t>
-  </si>
-  <si>
-    <t>Iode (produits de contraste)</t>
-  </si>
-  <si>
-    <t>Piqûres d’abeilles</t>
-  </si>
-  <si>
-    <t>Piqûres de guêpes</t>
-  </si>
-  <si>
-    <t>Piqûres de frelons</t>
-  </si>
-  <si>
-    <t>Latex</t>
   </si>
   <si>
     <t>Nickel</t>
@@ -100,22 +97,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color auto="1"/>
+      <family val="1"/>
+      <sz val="10"/>
+      <name val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,27 +121,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -155,15 +135,23 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -242,6 +230,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -276,6 +265,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -310,20 +300,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -445,20 +431,59 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B121"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="2" width="9.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,167 +491,268 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="10" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="14" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" ht="22.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="22.8" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>